<commit_message>
Add TS/PI features, POWER_QUERY docs, tests, and gitignore updates
- Add docs/POWER_QUERY.md (Power Query integration guide)
- Add packing_list template, analyze_sheets script
- Add tests for cli_common, config, excel_helpers
- Update generators with batch optimization and bug fixes
- Update .gitignore to exclude business data and company images

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/templates/proforma_invoice.xlsx
+++ b/templates/proforma_invoice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rotork-my.sharepoint.com/personal/jeongtaek_bang_rotork_com/Documents/바탕 화면/업무/NOAH ACTUATION/noahAutomation/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_715F5A10375D2708990628822A213EB7F6C545CC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A1E6A04-8E08-45E5-B59D-35696AD86995}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="11_715F5A10375D2708990628822A213EB7F6C545CC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8098FC14-258A-4C9A-B484-39291C2280FB}"/>
   <bookViews>
-    <workbookView xWindow="-1305" yWindow="-21720" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <r>
       <rPr>
@@ -78,28 +78,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Parts of actuator</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>EX-WORKS</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t>Total</t>
     </r>
   </si>
@@ -170,23 +148,11 @@
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
-    <t>UPS</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">From  : </t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>To       :</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">INCHEON </t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t>U.S.A.</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
@@ -226,10 +192,6 @@
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
-    <t>8481.90.3000</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
     <t>515, 5th floor Leader’s Bldg, Jangmi-ro 42,</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
@@ -252,28 +214,6 @@
   </si>
   <si>
     <t>Tel : 82-31-768-8151  Fax: 82-31-768-8156</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t>* Shipping Mark *</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t>ABZ</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Case No :
-</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t>Made in Korea</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">PO No : 
-</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
@@ -300,6 +240,19 @@
   </si>
   <si>
     <t xml:space="preserve">HS CODE: </t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>FOB</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>Electric Actuator</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>For and on behalf of 
+Rotork Controls Korea Co., Ltd.</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
 </sst>
@@ -307,11 +260,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="177" formatCode="[$USD]\ 0.00"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+    <numFmt numFmtId="179" formatCode="#,##0.00_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -443,7 +397,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -608,6 +562,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -616,7 +590,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -626,39 +600,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="3" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="3" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -674,12 +621,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -689,33 +630,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="3" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -731,8 +660,35 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="19" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="19" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
@@ -773,6 +729,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -809,12 +771,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -845,10 +801,10 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -857,10 +813,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -878,13 +831,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -896,14 +843,59 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="3" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="3" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -968,6 +960,56 @@
         <a:xfrm>
           <a:off x="132522" y="29472"/>
           <a:ext cx="1446696" cy="902182"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>33130</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>99391</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>55278</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{886DB268-BAAD-FB28-BC33-24494C9DF27D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6584673"/>
+          <a:ext cx="2087217" cy="800714"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1269,14 +1311,14 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="10.5" customWidth="1"/>
     <col min="2" max="2" width="5.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
@@ -1287,15 +1329,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A1" s="52"/>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
+      <c r="A1" s="48"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="30.75" customHeight="1">
@@ -1303,12 +1345,12 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="61" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
+      <c r="E2" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
@@ -1325,582 +1367,563 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="36" t="s">
+      <c r="A4" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="20"/>
+      <c r="H4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="20"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="16"/>
+      <c r="H5" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="16"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="35"/>
-      <c r="H4" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" s="35"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="63" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="36" t="s">
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="77" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A8" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" ht="33.6" customHeight="1">
+      <c r="A9" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" ht="13.5" customHeight="1">
+      <c r="A10" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A11" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="I5" s="30"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="48" t="s">
+      <c r="B11" s="72"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="43"/>
+      <c r="H11" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="39"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A12" s="67"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="84" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="85"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="68"/>
-      <c r="H7" s="68"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" ht="17.100000000000001" customHeight="1">
-      <c r="A8" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="68"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" ht="33.6" customHeight="1">
-      <c r="A9" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A10" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="25" t="s">
+      <c r="B13" s="75"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="G13" s="53"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="75"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="71"/>
-      <c r="H10" s="71"/>
-      <c r="I10" s="72"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A11" s="53" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="78"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="78"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="49"/>
-      <c r="H11" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A12" s="73" t="s">
+      <c r="G14" s="55"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" ht="17.850000000000001" customHeight="1">
+      <c r="A15" s="74" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="70">
+        <v>46030</v>
+      </c>
+      <c r="E15" s="71"/>
+      <c r="F15" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="74"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="37" t="s">
+      <c r="G15" s="27"/>
+      <c r="H15" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="82" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="83"/>
-      <c r="F13" s="56" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="57"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="37" t="s">
+      <c r="I15" s="29"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" ht="17.25" customHeight="1">
+      <c r="A16" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="80"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="31"/>
+      <c r="G16" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="82" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="82"/>
-      <c r="D14" s="82"/>
-      <c r="E14" s="83"/>
-      <c r="F14" s="58" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="59"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" ht="17.850000000000001" customHeight="1">
-      <c r="A15" s="80" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="81"/>
-      <c r="C15" s="81"/>
-      <c r="D15" s="76">
-        <v>46030</v>
-      </c>
-      <c r="E15" s="77"/>
-      <c r="F15" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="24"/>
-      <c r="H15" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15" s="32"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A16" s="89" t="s">
+      <c r="H16" s="30"/>
+      <c r="I16" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="89"/>
-      <c r="C16" s="89"/>
-      <c r="D16" s="89"/>
-      <c r="E16" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="15"/>
-      <c r="J16" s="14"/>
+      <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" ht="21" customHeight="1">
-      <c r="A17" s="54" t="s">
+      <c r="A17" s="86" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="86"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="88" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="89"/>
+      <c r="I17" s="90"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" ht="22.5" customHeight="1">
+      <c r="A18" s="91"/>
+      <c r="B18" s="91"/>
+      <c r="C18" s="91"/>
+      <c r="D18" s="91"/>
+      <c r="E18" s="92"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="93"/>
+      <c r="H18" s="94"/>
+      <c r="I18" s="95"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" ht="14.1" customHeight="1">
+      <c r="A19" s="91"/>
+      <c r="B19" s="91"/>
+      <c r="C19" s="91"/>
+      <c r="D19" s="91"/>
+      <c r="E19" s="92"/>
+      <c r="F19" s="87"/>
+      <c r="G19" s="93"/>
+      <c r="H19" s="94"/>
+      <c r="I19" s="95"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" customHeight="1">
+      <c r="A20" s="91"/>
+      <c r="B20" s="91"/>
+      <c r="C20" s="91"/>
+      <c r="D20" s="91"/>
+      <c r="E20" s="92"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="93"/>
+      <c r="H20" s="94"/>
+      <c r="I20" s="95"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" ht="14.1" customHeight="1">
+      <c r="A21" s="91"/>
+      <c r="B21" s="91"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="92"/>
+      <c r="F21" s="87"/>
+      <c r="G21" s="93"/>
+      <c r="H21" s="94"/>
+      <c r="I21" s="95"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" ht="14.1" customHeight="1">
+      <c r="A22" s="91"/>
+      <c r="B22" s="91"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="91"/>
+      <c r="E22" s="92"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="93"/>
+      <c r="H22" s="94"/>
+      <c r="I22" s="95"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" ht="14.1" customHeight="1">
+      <c r="A23" s="91"/>
+      <c r="B23" s="91"/>
+      <c r="C23" s="91"/>
+      <c r="D23" s="91"/>
+      <c r="E23" s="92"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="93"/>
+      <c r="H23" s="94"/>
+      <c r="I23" s="95"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" ht="15" customHeight="1">
+      <c r="A24" s="91"/>
+      <c r="B24" s="91"/>
+      <c r="C24" s="91"/>
+      <c r="D24" s="91"/>
+      <c r="E24" s="92"/>
+      <c r="F24" s="87"/>
+      <c r="G24" s="93"/>
+      <c r="H24" s="94"/>
+      <c r="I24" s="95"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" ht="15" customHeight="1">
+      <c r="A25" s="96"/>
+      <c r="B25" s="96"/>
+      <c r="C25" s="96"/>
+      <c r="D25" s="96"/>
+      <c r="E25" s="97"/>
+      <c r="F25" s="98"/>
+      <c r="G25" s="99"/>
+      <c r="H25" s="100"/>
+      <c r="I25" s="101"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" ht="22.5" customHeight="1">
+      <c r="A26" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="54"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" ht="22.5" customHeight="1">
-      <c r="A18" s="87"/>
-      <c r="B18" s="87"/>
-      <c r="C18" s="87"/>
-      <c r="D18" s="87"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" ht="14.1" customHeight="1">
-      <c r="A19" s="87"/>
-      <c r="B19" s="87"/>
-      <c r="C19" s="87"/>
-      <c r="D19" s="87"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1">
-      <c r="A20" s="87"/>
-      <c r="B20" s="87"/>
-      <c r="C20" s="87"/>
-      <c r="D20" s="87"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" ht="14.1" customHeight="1">
-      <c r="A21" s="87"/>
-      <c r="B21" s="87"/>
-      <c r="C21" s="87"/>
-      <c r="D21" s="87"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" ht="14.1" customHeight="1">
-      <c r="A22" s="87"/>
-      <c r="B22" s="87"/>
-      <c r="C22" s="87"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" ht="14.1" customHeight="1">
-      <c r="A23" s="87"/>
-      <c r="B23" s="87"/>
-      <c r="C23" s="87"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10" ht="15" customHeight="1">
-      <c r="A24" s="87"/>
-      <c r="B24" s="87"/>
-      <c r="C24" s="87"/>
-      <c r="D24" s="87"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10" ht="15" customHeight="1">
-      <c r="A25" s="88"/>
-      <c r="B25" s="88"/>
-      <c r="C25" s="88"/>
-      <c r="D25" s="88"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10" ht="22.5" customHeight="1">
-      <c r="A26" s="60" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="60"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="28">
+      <c r="B26" s="56"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="15">
         <f>SUM(E18:E25)</f>
         <v>0</v>
       </c>
-      <c r="F26" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G26" s="22"/>
-      <c r="H26" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="I26" s="38">
+      <c r="F26" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="11"/>
+      <c r="H26" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I26" s="23">
         <f>SUM(I18:I25)</f>
         <v>0</v>
       </c>
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="18" customHeight="1">
-      <c r="A27" s="65" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="65"/>
-      <c r="C27" s="65"/>
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="65"/>
-      <c r="J27" s="14"/>
+      <c r="A27" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="47"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="47"/>
+      <c r="J27" s="5"/>
     </row>
     <row r="28" spans="1:10" ht="18" customHeight="1">
-      <c r="A28" s="34"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="14"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="5"/>
     </row>
     <row r="29" spans="1:10" ht="18" customHeight="1">
-      <c r="A29" s="64" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="64"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="64"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="14"/>
-    </row>
-    <row r="30" spans="1:10" ht="18" customHeight="1" thickBot="1">
-      <c r="A30" s="64" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="64"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="14"/>
+      <c r="A29" s="46"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="5"/>
+    </row>
+    <row r="30" spans="1:10" ht="33" customHeight="1" thickBot="1">
+      <c r="A30" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="5"/>
     </row>
     <row r="31" spans="1:10" ht="18" customHeight="1">
-      <c r="A31" s="93" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" s="93"/>
-      <c r="C31" s="93"/>
-      <c r="D31" s="93"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="14"/>
+      <c r="A31" s="24"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
     </row>
     <row r="32" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A32" s="94" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" s="94"/>
-      <c r="C32" s="94">
-        <v>8116409</v>
-      </c>
-      <c r="D32" s="94"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="17"/>
+      <c r="A32" s="84"/>
+      <c r="B32" s="84"/>
+      <c r="C32" s="84"/>
+      <c r="D32" s="84"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="8"/>
     </row>
     <row r="33" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A33" s="94" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="94"/>
-      <c r="C33" s="95"/>
-      <c r="D33" s="95"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="17"/>
+      <c r="A33" s="84"/>
+      <c r="B33" s="84"/>
+      <c r="C33" s="85"/>
+      <c r="D33" s="85"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="8"/>
     </row>
     <row r="34" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A34" s="94" t="s">
-        <v>39</v>
-      </c>
-      <c r="B34" s="94"/>
-      <c r="C34" s="64"/>
-      <c r="D34" s="64"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="17"/>
+      <c r="A34" s="84"/>
+      <c r="B34" s="84"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="8"/>
     </row>
     <row r="35" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A35" s="31"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="17"/>
+      <c r="A35" s="17"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="8"/>
     </row>
     <row r="36" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A36" s="31"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="17"/>
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="8"/>
     </row>
     <row r="37" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A37" s="31"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="17"/>
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="8"/>
     </row>
     <row r="38" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A38" s="31"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="17"/>
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="8"/>
     </row>
     <row r="39" spans="1:10" ht="36" customHeight="1">
-      <c r="A39" s="90" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" s="90"/>
-      <c r="C39" s="90"/>
-      <c r="D39" s="90"/>
-      <c r="E39" s="90"/>
-      <c r="F39" s="90"/>
-      <c r="G39" s="90"/>
-      <c r="H39" s="90"/>
-      <c r="I39" s="90"/>
-      <c r="J39" s="17"/>
+      <c r="A39" s="81" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" s="81"/>
+      <c r="C39" s="81"/>
+      <c r="D39" s="81"/>
+      <c r="E39" s="81"/>
+      <c r="F39" s="81"/>
+      <c r="G39" s="81"/>
+      <c r="H39" s="81"/>
+      <c r="I39" s="81"/>
+      <c r="J39" s="8"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="91" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" s="91"/>
-      <c r="C40" s="91"/>
-      <c r="D40" s="91"/>
-      <c r="E40" s="91"/>
-      <c r="F40" s="92" t="s">
-        <v>43</v>
-      </c>
-      <c r="G40" s="92"/>
-      <c r="H40" s="92"/>
-      <c r="I40" s="92"/>
-      <c r="J40" s="18"/>
+      <c r="A40" s="82" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="82"/>
+      <c r="C40" s="82"/>
+      <c r="D40" s="82"/>
+      <c r="E40" s="82"/>
+      <c r="F40" s="83" t="s">
+        <v>32</v>
+      </c>
+      <c r="G40" s="83"/>
+      <c r="H40" s="83"/>
+      <c r="I40" s="83"/>
+      <c r="J40" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="45">
+  <mergeCells count="44">
     <mergeCell ref="A39:I39"/>
     <mergeCell ref="A40:E40"/>
     <mergeCell ref="F40:I40"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C34:D34"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A27:I27"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F7:I10"/>
     <mergeCell ref="A12:E12"/>
@@ -1910,22 +1933,21 @@
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A30:D30"/>
     <mergeCell ref="A9:E9"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="I11:I14"/>
     <mergeCell ref="F11:G12"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A25:D25"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F40" r:id="rId1" xr:uid="{DA519E99-AB88-496A-A4F0-AD3EE0BAD2E1}"/>
   </hyperlinks>
-  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <headerFooter>
     <oddFooter>&amp;CPage &amp;P of &amp;N</oddFooter>

</xml_diff>